<commit_message>
adding some YAASS chapman scores
</commit_message>
<xml_diff>
--- a/raw.xlsx
+++ b/raw.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3760" yWindow="820" windowWidth="15760" windowHeight="17360" tabRatio="500"/>
+    <workbookView xWindow="-320" yWindow="700" windowWidth="21440" windowHeight="20160" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -465,13 +465,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AD26" sqref="AD26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R73" sqref="R73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="14" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" customWidth="1"/>
+    <col min="3" max="14" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="15" max="15" width="17.1640625" customWidth="1"/>
     <col min="16" max="16" width="16.6640625" customWidth="1"/>
     <col min="17" max="17" width="17.6640625" customWidth="1"/>
@@ -581,7 +582,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>18</v>
       </c>
@@ -642,7 +643,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
@@ -733,7 +734,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -824,7 +825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -915,7 +916,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>18</v>
       </c>
@@ -1004,7 +1005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
@@ -1095,7 +1096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -1186,7 +1187,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>18</v>
       </c>
@@ -1277,7 +1278,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>18</v>
       </c>
@@ -1459,7 +1460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>18</v>
       </c>
@@ -1550,7 +1551,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
@@ -1641,7 +1642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>18</v>
       </c>
@@ -1732,7 +1733,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>18</v>
       </c>
@@ -1819,7 +1820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>18</v>
       </c>
@@ -1906,7 +1907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
@@ -2070,7 +2071,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -2157,7 +2158,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2244,7 +2245,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2323,7 +2324,7 @@
       <c r="AD21" s="1"/>
       <c r="AE21" s="1"/>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>19</v>
       </c>
@@ -2402,7 +2403,7 @@
       <c r="AD22" s="1"/>
       <c r="AE22" s="1"/>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2482,7 @@
       <c r="AD23" s="1"/>
       <c r="AE23" s="1"/>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>19</v>
       </c>
@@ -2552,7 +2553,7 @@
       <c r="AD24" s="1"/>
       <c r="AE24" s="1"/>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>19</v>
       </c>
@@ -2631,7 +2632,7 @@
       <c r="AD25" s="1"/>
       <c r="AE25" s="1"/>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>19</v>
       </c>
@@ -2684,7 +2685,7 @@
       <c r="AD26" s="1"/>
       <c r="AE26" s="1"/>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2763,7 +2764,7 @@
       <c r="AD27" s="1"/>
       <c r="AE27" s="1"/>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>19</v>
       </c>
@@ -2842,7 +2843,7 @@
       <c r="AD28" s="1"/>
       <c r="AE28" s="1"/>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>19</v>
       </c>
@@ -2921,7 +2922,7 @@
       <c r="AD29" s="1"/>
       <c r="AE29" s="1"/>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>19</v>
       </c>
@@ -3000,7 +3001,7 @@
       <c r="AD30" s="1"/>
       <c r="AE30" s="1"/>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>19</v>
       </c>
@@ -3067,7 +3068,7 @@
       <c r="AD31" s="1"/>
       <c r="AE31" s="1"/>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>19</v>
       </c>
@@ -3146,7 +3147,7 @@
       <c r="AD32" s="1"/>
       <c r="AE32" s="1"/>
     </row>
-    <row r="33" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>19</v>
       </c>
@@ -3217,7 +3218,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>19</v>
       </c>
@@ -3288,7 +3289,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="35" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>19</v>
       </c>
@@ -3355,7 +3356,7 @@
       <c r="AA35" s="2"/>
       <c r="AB35" s="2"/>
     </row>
-    <row r="36" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>19</v>
       </c>
@@ -3426,7 +3427,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>19</v>
       </c>
@@ -3497,7 +3498,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
         <v>19</v>
       </c>
@@ -3568,7 +3569,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
         <v>19</v>
       </c>
@@ -3637,7 +3638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
         <v>19</v>
       </c>
@@ -3708,7 +3709,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
         <v>19</v>
       </c>
@@ -3779,7 +3780,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
         <v>19</v>
       </c>
@@ -3850,7 +3851,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="43" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
         <v>19</v>
       </c>
@@ -3921,7 +3922,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="44" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
         <v>19</v>
       </c>
@@ -3992,7 +3993,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="45" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>19</v>
       </c>
@@ -4063,7 +4064,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>19</v>
       </c>
@@ -4134,7 +4135,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="47" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
         <v>20</v>
       </c>
@@ -4205,7 +4206,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="48" spans="1:28" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:28" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
         <v>20</v>
       </c>
@@ -4276,7 +4277,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
         <v>20</v>
       </c>
@@ -4339,7 +4340,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="50" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -4410,7 +4411,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -4481,7 +4482,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="52" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
         <v>20</v>
       </c>
@@ -4552,7 +4553,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
         <v>20</v>
       </c>
@@ -4615,7 +4616,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="54" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
         <v>20</v>
       </c>
@@ -4686,7 +4687,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
         <v>20</v>
       </c>
@@ -4757,7 +4758,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="56" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
         <v>20</v>
       </c>
@@ -4828,7 +4829,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="57" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
         <v>20</v>
       </c>
@@ -4899,7 +4900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
         <v>20</v>
       </c>
@@ -4970,7 +4971,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
         <v>20</v>
       </c>
@@ -5041,7 +5042,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="60" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" s="1" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
         <v>20</v>
       </c>
@@ -5835,10 +5836,18 @@
       <c r="N71" s="1">
         <v>2.1544900626799999</v>
       </c>
-      <c r="O71" s="2"/>
-      <c r="P71" s="2"/>
-      <c r="Q71" s="2"/>
-      <c r="S71" s="2"/>
+      <c r="O71" s="1">
+        <v>8</v>
+      </c>
+      <c r="P71" s="1">
+        <v>7</v>
+      </c>
+      <c r="Q71" s="1">
+        <v>5</v>
+      </c>
+      <c r="S71" s="1">
+        <v>3</v>
+      </c>
       <c r="U71" s="1">
         <v>1</v>
       </c>
@@ -5908,9 +5917,15 @@
       <c r="N72" s="1">
         <v>0.83758827156000004</v>
       </c>
-      <c r="O72" s="2"/>
-      <c r="P72" s="2"/>
-      <c r="Q72" s="2"/>
+      <c r="O72" s="1">
+        <v>0</v>
+      </c>
+      <c r="P72" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q72" s="1">
+        <v>0</v>
+      </c>
       <c r="S72" s="2"/>
       <c r="U72" s="1">
         <v>0</v>
@@ -6046,9 +6061,15 @@
       <c r="N74" s="1">
         <v>1.9898773387899999</v>
       </c>
-      <c r="O74" s="2"/>
-      <c r="P74" s="2"/>
-      <c r="Q74" s="2"/>
+      <c r="O74" s="1">
+        <v>0</v>
+      </c>
+      <c r="P74" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q74" s="1">
+        <v>0</v>
+      </c>
       <c r="S74" s="2"/>
       <c r="U74" s="1">
         <v>0</v>
@@ -6196,9 +6217,15 @@
       <c r="N76" s="1">
         <v>0.83758827156000004</v>
       </c>
-      <c r="O76" s="2"/>
-      <c r="P76" s="2"/>
-      <c r="Q76" s="2"/>
+      <c r="O76" s="1">
+        <v>0</v>
+      </c>
+      <c r="P76" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q76" s="1">
+        <v>0</v>
+      </c>
       <c r="S76" s="2"/>
       <c r="U76" s="1">
         <v>1</v>
@@ -6271,9 +6298,15 @@
       <c r="N77" s="1">
         <v>1.4524652108E-2</v>
       </c>
-      <c r="O77" s="2"/>
-      <c r="P77" s="2"/>
-      <c r="Q77" s="2"/>
+      <c r="O77" s="1">
+        <v>0</v>
+      </c>
+      <c r="P77" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q77" s="1">
+        <v>0</v>
+      </c>
       <c r="S77" s="2"/>
       <c r="U77" s="1">
         <v>0</v>
@@ -6636,9 +6669,11 @@
       <c r="N82" s="1">
         <v>1.49603916712</v>
       </c>
-      <c r="O82" s="2"/>
+      <c r="O82" s="1">
+        <v>0</v>
+      </c>
       <c r="P82" s="1">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Q82" s="1">
         <v>0</v>
@@ -6872,7 +6907,9 @@
       <c r="Q85" s="1">
         <v>13</v>
       </c>
-      <c r="S85" s="2"/>
+      <c r="S85" s="1">
+        <v>18</v>
+      </c>
       <c r="U85" s="1">
         <v>1</v>
       </c>
@@ -7026,7 +7063,9 @@
       <c r="Q87" s="1">
         <v>10</v>
       </c>
-      <c r="S87" s="2"/>
+      <c r="S87" s="1">
+        <v>12</v>
+      </c>
       <c r="U87" s="1">
         <v>2</v>
       </c>
@@ -7184,7 +7223,9 @@
       <c r="Q89" s="1">
         <v>6</v>
       </c>
-      <c r="S89" s="2"/>
+      <c r="S89" s="1">
+        <v>9</v>
+      </c>
       <c r="U89" s="1">
         <v>2</v>
       </c>
@@ -7662,7 +7703,9 @@
       <c r="Q95" s="1">
         <v>0</v>
       </c>
-      <c r="S95" s="2"/>
+      <c r="S95" s="1">
+        <v>5</v>
+      </c>
       <c r="U95" s="1">
         <v>0</v>
       </c>
@@ -7823,7 +7866,9 @@
         <v>7</v>
       </c>
       <c r="R97" s="1"/>
-      <c r="S97" s="2"/>
+      <c r="S97" s="1">
+        <v>34</v>
+      </c>
       <c r="T97" s="1"/>
       <c r="U97" s="1">
         <v>7</v>
@@ -7906,7 +7951,9 @@
         <v>6</v>
       </c>
       <c r="R98" s="1"/>
-      <c r="S98" s="2"/>
+      <c r="S98" s="1">
+        <v>13</v>
+      </c>
       <c r="T98" s="1"/>
       <c r="U98" s="1">
         <v>3</v>
@@ -8368,7 +8415,9 @@
         <v>11</v>
       </c>
       <c r="R104" s="1"/>
-      <c r="S104" s="2"/>
+      <c r="S104" s="1">
+        <v>31</v>
+      </c>
       <c r="T104" s="1"/>
       <c r="U104" s="1">
         <v>2</v>
@@ -8520,9 +8569,15 @@
       <c r="N106" s="1">
         <v>-1.46698986291</v>
       </c>
-      <c r="O106" s="2"/>
-      <c r="P106" s="2"/>
-      <c r="Q106" s="2"/>
+      <c r="O106" s="1">
+        <v>17</v>
+      </c>
+      <c r="P106" s="1">
+        <v>6</v>
+      </c>
+      <c r="Q106" s="1">
+        <v>6</v>
+      </c>
       <c r="R106" s="1"/>
       <c r="S106" s="1">
         <v>36</v>
@@ -8800,9 +8855,15 @@
       <c r="N110" s="1">
         <v>1.33142644323</v>
       </c>
-      <c r="O110" s="2"/>
-      <c r="P110" s="2"/>
-      <c r="Q110" s="2"/>
+      <c r="O110" s="1">
+        <v>27</v>
+      </c>
+      <c r="P110" s="1">
+        <v>18</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>15</v>
+      </c>
       <c r="R110" s="1"/>
       <c r="S110" s="2"/>
       <c r="T110" s="1"/>

</xml_diff>